<commit_message>
Convert status options to concise English and add Acknowledged status
</commit_message>
<xml_diff>
--- a/templates/mailsToFlow1.xlsx
+++ b/templates/mailsToFlow1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwrwnlwy/projects/anomalies/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E133169-DBC8-B141-9E0F-6AE8F7A321AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB53C57-BF81-3B4E-BAD4-6B655E9DBF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18000" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="341">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -703,9 +703,6 @@
     <t>treetoscope.com</t>
   </si>
   <si>
-    <t>keren.h@treetoscope.com;alon.fux@treetoscope.com</t>
-  </si>
-  <si>
     <t>TreeToScope team</t>
   </si>
   <si>
@@ -715,9 +712,6 @@
     <t>shlomo-sixt-sandbox</t>
   </si>
   <si>
-    <t>leond@shlomo.co.il;igorh@shlomo.co.il</t>
-  </si>
-  <si>
     <t>Igor and Leonid</t>
   </si>
   <si>
@@ -1046,6 +1040,9 @@
   </si>
   <si>
     <t>yossi@tracklease.com</t>
+  </si>
+  <si>
+    <t>Leonidg@Shlomo.co.il;igorh@shlomo.co.il</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2743,77 +2740,77 @@
         <v>226</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E97" t="s">
         <v>227</v>
-      </c>
-      <c r="E97" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C98" t="s">
         <v>229</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E98" t="s">
         <v>230</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E98" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>231</v>
+        <v>340</v>
       </c>
       <c r="E99" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C100" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>231</v>
+        <v>340</v>
       </c>
       <c r="E100" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C101" t="s">
+        <v>236</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C101" t="s">
+      <c r="E101" t="s">
         <v>238</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E101" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" t="s">
+        <v>240</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C102" t="s">
-        <v>242</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="E102" t="s">
         <v>115</v>
@@ -2821,186 +2818,186 @@
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C103" t="s">
+        <v>243</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C103" t="s">
+      <c r="E103" t="s">
         <v>245</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E103" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C104" t="s">
+        <v>247</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C104" t="s">
+      <c r="E104" t="s">
         <v>249</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E104" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C105" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C106" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B107" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C107" t="s">
+        <v>255</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C107" t="s">
+      <c r="E107" t="s">
         <v>257</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E107" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C108" t="s">
+        <v>259</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C108" t="s">
+      <c r="E108" t="s">
         <v>261</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E108" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C109" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B110" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C110" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C110" t="s">
+      <c r="E110" t="s">
         <v>267</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E110" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B111" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C111" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E111" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C112" t="s">
+        <v>271</v>
+      </c>
+      <c r="D112" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C112" t="s">
+      <c r="E112" t="s">
         <v>273</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E112" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C113" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E113" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C114" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C115" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C116" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C117" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B118" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C118" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>60</v>
@@ -3011,185 +3008,185 @@
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C120" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C121" t="s">
+        <v>291</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C121" t="s">
+      <c r="E121" t="s">
         <v>293</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="F121" t="s">
         <v>294</v>
-      </c>
-      <c r="E121" t="s">
-        <v>295</v>
-      </c>
-      <c r="F121" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C122" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E122" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C123" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E123" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C124" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E124" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C125" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E125" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C126" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E126" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C127" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C128" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B129" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C129" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B130" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C130" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C131" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B132" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C132" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B133" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C133" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B134" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C134" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B135" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C135" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B136" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C136" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B137" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C137" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -3197,40 +3194,40 @@
         <v>195</v>
       </c>
       <c r="C138" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B139" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C139" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B140" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C140" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B141" s="5">
         <v>170744924094</v>
       </c>
       <c r="C141" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E141" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -3238,13 +3235,13 @@
         <v>728009587795</v>
       </c>
       <c r="C142" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E142" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3252,13 +3249,13 @@
         <v>941677598037</v>
       </c>
       <c r="C143" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E143" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3266,13 +3263,13 @@
         <v>579201838494</v>
       </c>
       <c r="C144" t="s">
+        <v>337</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D144" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="E144" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.2">
@@ -3280,18 +3277,22 @@
         <v>560428933869</v>
       </c>
       <c r="C145" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E145" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D41" r:id="rId1" xr:uid="{DF273828-6A49-EA43-9335-A5EBEF245073}"/>
+    <hyperlink ref="D100" r:id="rId2" xr:uid="{329FED7F-47D1-3549-B2C9-0FA567100759}"/>
+    <hyperlink ref="D99" r:id="rId3" xr:uid="{0173A0A0-0FF5-1D4C-8BAE-411F0C33C93C}"/>
+    <hyperlink ref="D98" r:id="rId4" xr:uid="{15EA03BF-2AB5-BF44-9725-85693FCCA5C9}"/>
+    <hyperlink ref="D97" r:id="rId5" xr:uid="{F0EC2A9A-68A6-234C-BA5E-A838A525542A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>